<commit_message>
add esp12-f to r01 bom
</commit_message>
<xml_diff>
--- a/hardware/pcb/pi433_r01_bom.xlsx
+++ b/hardware/pcb/pi433_r01_bom.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/gitrepos/pi433/hardware/pcb/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22640" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="26600" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="132">
   <si>
     <t>UID</t>
   </si>
@@ -84,9 +92,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>PI433_00_01</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -330,54 +335,9 @@
     <t>RES SMD 10K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>PI433_00_02</t>
-  </si>
-  <si>
-    <t>PI433_00_03</t>
-  </si>
-  <si>
-    <t>PI433_00_04</t>
-  </si>
-  <si>
-    <t>PI433_00_05</t>
-  </si>
-  <si>
-    <t>PI433_00_06</t>
-  </si>
-  <si>
-    <t>PI433_00_07</t>
-  </si>
-  <si>
-    <t>PI433_00_08</t>
-  </si>
-  <si>
-    <t>PI433_00_09</t>
-  </si>
-  <si>
-    <t>PI433_00_10</t>
-  </si>
-  <si>
-    <t>PI433_00_11</t>
-  </si>
-  <si>
-    <t>PI433_00_12</t>
-  </si>
-  <si>
-    <t>PI433_00_13</t>
-  </si>
-  <si>
-    <t>PI433_00_14</t>
-  </si>
-  <si>
-    <t>PI433_00_15</t>
-  </si>
-  <si>
     <t>LED1, LED2, LED3, LED4</t>
   </si>
   <si>
-    <t>PI433_00_16</t>
-  </si>
-  <si>
     <t>160-1423-1-ND</t>
   </si>
   <si>
@@ -394,6 +354,75 @@
   </si>
   <si>
     <t>DIGIKEY ORDER 1/7/16</t>
+  </si>
+  <si>
+    <t>PI433_01_01</t>
+  </si>
+  <si>
+    <t>PI433_01_02</t>
+  </si>
+  <si>
+    <t>PI433_01_03</t>
+  </si>
+  <si>
+    <t>PI433_01_04</t>
+  </si>
+  <si>
+    <t>PI433_01_05</t>
+  </si>
+  <si>
+    <t>PI433_01_06</t>
+  </si>
+  <si>
+    <t>PI433_01_07</t>
+  </si>
+  <si>
+    <t>PI433_01_08</t>
+  </si>
+  <si>
+    <t>PI433_01_09</t>
+  </si>
+  <si>
+    <t>PI433_01_10</t>
+  </si>
+  <si>
+    <t>PI433_01_11</t>
+  </si>
+  <si>
+    <t>PI433_01_12</t>
+  </si>
+  <si>
+    <t>PI433_01_13</t>
+  </si>
+  <si>
+    <t>PI433_01_14</t>
+  </si>
+  <si>
+    <t>PI433_01_15</t>
+  </si>
+  <si>
+    <t>PI433_01_16</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>WIFI Transceiver</t>
+  </si>
+  <si>
+    <t>SDIO interface WiFi transceiver</t>
+  </si>
+  <si>
+    <t>ESP-12F</t>
+  </si>
+  <si>
+    <t>GearBest</t>
+  </si>
+  <si>
+    <t>Yison</t>
+  </si>
+  <si>
+    <t>PI433_01_17</t>
   </si>
 </sst>
 </file>
@@ -566,6 +595,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -894,10 +928,10 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -913,7 +947,7 @@
     <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,18 +985,18 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="N1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -971,13 +1005,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -986,7 +1020,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1003,12 +1037,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -1017,13 +1051,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -1032,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1049,12 +1083,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1063,13 +1097,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -1078,7 +1112,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1095,12 +1129,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1109,13 +1143,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -1124,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1141,12 +1175,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1155,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
@@ -1170,7 +1204,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1187,9 +1221,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1201,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
@@ -1216,7 +1250,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1233,12 +1267,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -1247,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -1262,7 +1296,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1279,12 +1313,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1293,13 +1327,13 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -1308,7 +1342,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1325,12 +1359,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -1339,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -1354,7 +1388,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1371,12 +1405,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -1385,13 +1419,13 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1400,7 +1434,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1417,36 +1451,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1463,36 +1497,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
         <v>53</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
       </c>
       <c r="I13" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1509,36 +1543,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" t="s">
         <v>64</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>67</v>
       </c>
-      <c r="G14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="J14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="I14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1551,12 +1585,12 @@
         <v>6.66</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1565,22 +1599,22 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
         <v>71</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" t="s">
-        <v>72</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1597,103 +1631,149 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="G16" t="s">
+        <v>128</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="I16" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0.56000000000000005</v>
+        <v>3.19</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>3.19</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M17">
+        <f>D17/K17*L17</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N17">
+        <f>D17/K17*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
+      <c r="M18">
+        <f>D18/K18*L18</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
+      <c r="N18">
+        <f>D18/K18*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
       <c r="H23" s="4"/>
@@ -1701,7 +1781,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
       <c r="H24" s="4"/>
@@ -1709,54 +1789,54 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="6:12">
+    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="6:12">
+    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
       <c r="H34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="6:12">
+    <row r="35" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="6:12">
+    <row r="36" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -1764,7 +1844,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="6:12">
+    <row r="37" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -1772,89 +1852,89 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="6:12">
+    <row r="38" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G38" s="1"/>
       <c r="H38" s="6"/>
       <c r="J38" s="1"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="6:12">
+    <row r="39" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="6:12">
+    <row r="40" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="6:12">
+    <row r="41" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="6:12">
+    <row r="42" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F42" s="2"/>
       <c r="G42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="6:12">
+    <row r="43" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="6:12">
+    <row r="44" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="6:12">
+    <row r="45" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="6:12">
+    <row r="46" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="6:12">
+    <row r="47" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="6:12">
+    <row r="48" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="2:10">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="2:10">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G51" s="1"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="2:10">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="2:10">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="2:10">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="2:10">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="2:10">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="7"/>
       <c r="G57" s="1"/>
       <c r="J57" s="1"/>
@@ -1871,8 +1951,8 @@
     <hyperlink ref="J14" r:id="rId8"/>
     <hyperlink ref="J15" r:id="rId9"/>
     <hyperlink ref="G15" r:id="rId10"/>
-    <hyperlink ref="G16" r:id="rId11"/>
-    <hyperlink ref="J16" r:id="rId12"/>
+    <hyperlink ref="G17" r:id="rId11"/>
+    <hyperlink ref="J17" r:id="rId12"/>
     <hyperlink ref="J2" r:id="rId13"/>
     <hyperlink ref="G2" r:id="rId14"/>
     <hyperlink ref="J3" r:id="rId15"/>
@@ -1887,15 +1967,11 @@
     <hyperlink ref="G7" r:id="rId24"/>
     <hyperlink ref="J8" r:id="rId25"/>
     <hyperlink ref="G8" r:id="rId26"/>
-    <hyperlink ref="J17" r:id="rId27"/>
-    <hyperlink ref="G17" r:id="rId28"/>
+    <hyperlink ref="J18" r:id="rId27"/>
+    <hyperlink ref="G18" r:id="rId28"/>
+    <hyperlink ref="J16" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>